<commit_message>
added larger example, updated presentation
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Tony</t>
   </si>
@@ -36,43 +36,19 @@
     <t>Steve</t>
   </si>
   <si>
-    <t>Natasha</t>
-  </si>
-  <si>
-    <t>Wanda</t>
-  </si>
-  <si>
-    <t>Susan</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>1.3</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>2.5</t>
+    <t>Mon 28/02</t>
+  </si>
+  <si>
+    <t>Tue 01/03</t>
+  </si>
+  <si>
+    <t>Wed 02/03</t>
+  </si>
+  <si>
+    <t>Thu 03/03</t>
+  </si>
+  <si>
+    <t>Fri 04/03</t>
   </si>
 </sst>
 </file>
@@ -424,50 +400,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -476,36 +437,21 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -516,23 +462,8 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -549,126 +480,6 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
         <v>0</v>
       </c>
     </row>

</xml_diff>